<commit_message>
added support for changing reaction and total volume
</commit_message>
<xml_diff>
--- a/source_plates/ECHO_source_plate_dummy.xlsx
+++ b/source_plates/ECHO_source_plate_dummy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carothers4/Documents/GitHub/WHISPR/source_plates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rycar\Documents\GitHub\WHISPR\source_plates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FBE25E-5496-9E45-87EB-CB711135C953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB60338C-4D78-44E1-B5F7-AA6D1907DCB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3280" yWindow="7620" windowWidth="37360" windowHeight="21100" xr2:uid="{546D7F41-76BF-4117-BD41-03A67E651BAB}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{546D7F41-76BF-4117-BD41-03A67E651BAB}"/>
   </bookViews>
   <sheets>
     <sheet name="ECHO_source_plate" sheetId="1" r:id="rId1"/>
@@ -84,40 +84,40 @@
     <t>pRC008.206_10000x</t>
   </si>
   <si>
-    <t>A1,A2,A3,A4,A5,A6,A7,A8,A9,A10,A11,A12</t>
-  </si>
-  <si>
-    <t>65,65,65,65,65,65,65,65,65,65,65,65</t>
-  </si>
-  <si>
-    <t>B3</t>
-  </si>
-  <si>
-    <t>B4</t>
-  </si>
-  <si>
-    <t>B5</t>
-  </si>
-  <si>
-    <t>B6</t>
-  </si>
-  <si>
-    <t>B7</t>
-  </si>
-  <si>
-    <t>B8</t>
-  </si>
-  <si>
-    <t>B9</t>
-  </si>
-  <si>
-    <t>B10</t>
-  </si>
-  <si>
-    <t>B11</t>
-  </si>
-  <si>
-    <t>B12</t>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>A9</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>65,65</t>
+  </si>
+  <si>
+    <t>A11,A12</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
   </si>
 </sst>
 </file>
@@ -494,17 +494,17 @@
   <dimension ref="A1:Y16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.5" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="5" width="15.5" customWidth="1"/>
+    <col min="1" max="1" width="11.47265625" customWidth="1"/>
+    <col min="2" max="2" width="20.68359375" customWidth="1"/>
+    <col min="3" max="5" width="15.47265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -541,7 +541,7 @@
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -549,10 +549,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -575,7 +575,7 @@
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -583,7 +583,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D3">
         <v>222</v>
@@ -612,7 +612,7 @@
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -620,7 +620,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D4">
         <v>2.2200000000000002</v>
@@ -649,7 +649,7 @@
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -657,7 +657,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D5">
         <v>0.22</v>
@@ -686,7 +686,7 @@
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -694,7 +694,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D6">
         <v>199.76</v>
@@ -723,7 +723,7 @@
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D7">
         <v>201.96</v>
@@ -760,7 +760,7 @@
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -768,7 +768,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D8">
         <v>126.77</v>
@@ -797,7 +797,7 @@
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -805,7 +805,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D9">
         <v>164.65</v>
@@ -834,7 +834,7 @@
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -842,7 +842,7 @@
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D10">
         <v>16.465</v>
@@ -871,7 +871,7 @@
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -879,7 +879,7 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D11">
         <v>0.16464999999999999</v>
@@ -908,7 +908,7 @@
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -916,7 +916,7 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D12">
         <v>1.6465E-2</v>
@@ -945,7 +945,7 @@
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -971,7 +971,7 @@
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -997,7 +997,7 @@
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1023,7 +1023,7 @@
       <c r="X15" s="1"/>
       <c r="Y15" s="1"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>

</xml_diff>